<commit_message>
adc to get_instance style, figure multi type reading
</commit_message>
<xml_diff>
--- a/workspace/bluepill-proto/Calculations.xlsx
+++ b/workspace/bluepill-proto/Calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Documents\Git\RT_soldering_pen\workspace\bluepill-proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF701A0-0C2B-4733-ABD6-73A8A500E660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F6FEE3-CF10-4239-816A-0F7C3BEC7697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27105" yWindow="5475" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{1DE8D587-94D3-402A-AB86-DAC758A4112A}"/>
+    <workbookView xWindow="-28920" yWindow="3405" windowWidth="29040" windowHeight="15990" xr2:uid="{1DE8D587-94D3-402A-AB86-DAC758A4112A}"/>
   </bookViews>
   <sheets>
     <sheet name="ADC timing" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="45">
   <si>
     <t xml:space="preserve">ADC Clock </t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>bits</t>
+  </si>
+  <si>
+    <t>ARR</t>
+  </si>
+  <si>
+    <t>Figuring out the timing to use for PWM 2.</t>
+  </si>
+  <si>
+    <t>We want 20Hz? With breakouts for dead time and heat/measure</t>
   </si>
 </sst>
 </file>
@@ -575,12 +584,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F180A47B-38DB-47FC-A639-5EBFCAC3A986}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -814,10 +824,12 @@
       <c r="H21" s="3">
         <v>6</v>
       </c>
+      <c r="I21" s="3">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
-        <f>D14</f>
         <v>7</v>
       </c>
       <c r="B22" s="3">
@@ -828,7 +840,7 @@
         <v>7</v>
       </c>
       <c r="D22">
-        <f t="shared" ref="D22:H28" si="3">$B22*D$21*$A$22</f>
+        <f t="shared" ref="D22:I28" si="3">$B22*D$21*$A$22</f>
         <v>14</v>
       </c>
       <c r="E22">
@@ -844,8 +856,12 @@
         <v>35</v>
       </c>
       <c r="H22">
-        <f t="shared" si="3"/>
+        <f>$B22*H$21*$A$22</f>
         <v>42</v>
+      </c>
+      <c r="I22">
+        <f>$B22*I$21*$A$22</f>
+        <v>49</v>
       </c>
       <c r="J22" t="s">
         <v>10</v>
@@ -879,6 +895,10 @@
         <f t="shared" si="3"/>
         <v>84</v>
       </c>
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
@@ -908,6 +928,10 @@
         <f t="shared" si="3"/>
         <v>168</v>
       </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>196</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
@@ -937,6 +961,10 @@
         <f t="shared" si="3"/>
         <v>336</v>
       </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>392</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
@@ -966,6 +994,10 @@
         <f t="shared" si="3"/>
         <v>672</v>
       </c>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>784</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
@@ -995,6 +1027,10 @@
         <f t="shared" si="3"/>
         <v>1344</v>
       </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>1568</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
@@ -1023,6 +1059,10 @@
       <c r="H28">
         <f t="shared" si="3"/>
         <v>2688</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>3136</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2375,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1011573-8F2A-49B4-8E44-3335466A1B88}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2386,6 +2426,9 @@
     <col min="4" max="4" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2499,14 +2542,66 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B479DB4-E2D6-41EA-A30C-2398ACD29C2B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35:I37"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>48000000</v>
+      </c>
+      <c r="B7" s="2">
+        <v>480</v>
+      </c>
+      <c r="C7">
+        <f>A7/B7</f>
+        <v>100000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E7">
+        <f>C7/D7</f>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>